<commit_message>
feat: :sparkles: mod base concurso
</commit_message>
<xml_diff>
--- a/BASE-CONCURSO.xlsx
+++ b/BASE-CONCURSO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Sorteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788A7A85-4600-4E52-A68E-97D2B040231D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D863DBD-C522-456A-B156-E92845915878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8FFDBAC9-2DE9-408A-9BF2-928E062B7C63}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -331,15 +331,9 @@
     <t>Andrea Loayza</t>
   </si>
   <si>
-    <t>Alicia</t>
-  </si>
-  <si>
     <t>Isabel Parra</t>
   </si>
   <si>
-    <t>Ivaovva</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manuel Ordóñez </t>
   </si>
   <si>
@@ -421,9 +415,6 @@
     <t>Luis Emilio Veintimilla León</t>
   </si>
   <si>
-    <t>Ramiro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Karla Ponce </t>
   </si>
   <si>
@@ -449,9 +440,6 @@
   </si>
   <si>
     <t xml:space="preserve">Martín Fernando Randi Proaño </t>
-  </si>
-  <si>
-    <t>Andre R</t>
   </si>
   <si>
     <t xml:space="preserve">Daniela Zapata </t>
@@ -3368,10 +3356,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D65B54-0E84-42C0-8A01-31349AEC5EC7}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B63"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3426,7 +3414,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>259743</v>
+        <v>259741</v>
       </c>
       <c r="B7" t="s">
         <v>97</v>
@@ -3434,7 +3422,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>259741</v>
+        <v>259737</v>
       </c>
       <c r="B8" t="s">
         <v>98</v>
@@ -3442,7 +3430,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>259739</v>
+        <v>259735</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -3450,7 +3438,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>259737</v>
+        <v>259733</v>
       </c>
       <c r="B10" t="s">
         <v>100</v>
@@ -3458,7 +3446,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>259735</v>
+        <v>259731</v>
       </c>
       <c r="B11" t="s">
         <v>101</v>
@@ -3466,7 +3454,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>259733</v>
+        <v>259729</v>
       </c>
       <c r="B12" t="s">
         <v>102</v>
@@ -3474,7 +3462,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>259731</v>
+        <v>259727</v>
       </c>
       <c r="B13" t="s">
         <v>103</v>
@@ -3482,7 +3470,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>259729</v>
+        <v>259725</v>
       </c>
       <c r="B14" t="s">
         <v>104</v>
@@ -3490,7 +3478,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>259727</v>
+        <v>259723</v>
       </c>
       <c r="B15" t="s">
         <v>105</v>
@@ -3498,7 +3486,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>259725</v>
+        <v>259721</v>
       </c>
       <c r="B16" t="s">
         <v>106</v>
@@ -3506,7 +3494,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>259723</v>
+        <v>259719</v>
       </c>
       <c r="B17" t="s">
         <v>107</v>
@@ -3514,7 +3502,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>259721</v>
+        <v>259717</v>
       </c>
       <c r="B18" t="s">
         <v>108</v>
@@ -3522,7 +3510,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>259719</v>
+        <v>259715</v>
       </c>
       <c r="B19" t="s">
         <v>109</v>
@@ -3530,7 +3518,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>259717</v>
+        <v>259713</v>
       </c>
       <c r="B20" t="s">
         <v>110</v>
@@ -3538,7 +3526,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>259715</v>
+        <v>259711</v>
       </c>
       <c r="B21" t="s">
         <v>111</v>
@@ -3546,7 +3534,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>259713</v>
+        <v>259709</v>
       </c>
       <c r="B22" t="s">
         <v>112</v>
@@ -3554,7 +3542,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>259711</v>
+        <v>259707</v>
       </c>
       <c r="B23" t="s">
         <v>113</v>
@@ -3562,7 +3550,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>259709</v>
+        <v>259705</v>
       </c>
       <c r="B24" t="s">
         <v>114</v>
@@ -3570,7 +3558,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>259707</v>
+        <v>259703</v>
       </c>
       <c r="B25" t="s">
         <v>115</v>
@@ -3578,7 +3566,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>259705</v>
+        <v>259701</v>
       </c>
       <c r="B26" t="s">
         <v>116</v>
@@ -3586,7 +3574,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>259703</v>
+        <v>259699</v>
       </c>
       <c r="B27" t="s">
         <v>117</v>
@@ -3594,7 +3582,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>259701</v>
+        <v>259697</v>
       </c>
       <c r="B28" t="s">
         <v>118</v>
@@ -3602,39 +3590,39 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>259699</v>
+        <v>259695</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>259697</v>
+        <v>259693</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>259695</v>
+        <v>259691</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>259693</v>
+        <v>259689</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>259691</v>
+        <v>259681</v>
       </c>
       <c r="B33" t="s">
         <v>121</v>
@@ -3642,7 +3630,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>259689</v>
+        <v>259679</v>
       </c>
       <c r="B34" t="s">
         <v>122</v>
@@ -3650,7 +3638,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>259681</v>
+        <v>259645</v>
       </c>
       <c r="B35" t="s">
         <v>123</v>
@@ -3658,7 +3646,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>259679</v>
+        <v>259643</v>
       </c>
       <c r="B36" t="s">
         <v>124</v>
@@ -3666,7 +3654,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>259645</v>
+        <v>259639</v>
       </c>
       <c r="B37" t="s">
         <v>125</v>
@@ -3674,7 +3662,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>259643</v>
+        <v>259635</v>
       </c>
       <c r="B38" t="s">
         <v>126</v>
@@ -3682,7 +3670,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>259641</v>
+        <v>259633</v>
       </c>
       <c r="B39" t="s">
         <v>127</v>
@@ -3690,7 +3678,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>259639</v>
+        <v>259631</v>
       </c>
       <c r="B40" t="s">
         <v>128</v>
@@ -3698,7 +3686,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>259635</v>
+        <v>259627</v>
       </c>
       <c r="B41" t="s">
         <v>129</v>
@@ -3706,7 +3694,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>259633</v>
+        <v>259625</v>
       </c>
       <c r="B42" t="s">
         <v>130</v>
@@ -3714,7 +3702,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>259631</v>
+        <v>259623</v>
       </c>
       <c r="B43" t="s">
         <v>131</v>
@@ -3722,7 +3710,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>259627</v>
+        <v>259621</v>
       </c>
       <c r="B44" t="s">
         <v>132</v>
@@ -3730,7 +3718,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>259625</v>
+        <v>259619</v>
       </c>
       <c r="B45" t="s">
         <v>133</v>
@@ -3738,7 +3726,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>259623</v>
+        <v>259615</v>
       </c>
       <c r="B46" t="s">
         <v>134</v>
@@ -3746,7 +3734,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>259621</v>
+        <v>259613</v>
       </c>
       <c r="B47" t="s">
         <v>135</v>
@@ -3754,7 +3742,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>259619</v>
+        <v>259611</v>
       </c>
       <c r="B48" t="s">
         <v>136</v>
@@ -3762,7 +3750,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>259617</v>
+        <v>259609</v>
       </c>
       <c r="B49" t="s">
         <v>137</v>
@@ -3770,7 +3758,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>259615</v>
+        <v>259607</v>
       </c>
       <c r="B50" t="s">
         <v>138</v>
@@ -3778,7 +3766,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>259613</v>
+        <v>259605</v>
       </c>
       <c r="B51" t="s">
         <v>139</v>
@@ -3786,7 +3774,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>259611</v>
+        <v>259603</v>
       </c>
       <c r="B52" t="s">
         <v>140</v>
@@ -3794,7 +3782,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>259609</v>
+        <v>259601</v>
       </c>
       <c r="B53" t="s">
         <v>141</v>
@@ -3802,7 +3790,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>259607</v>
+        <v>259599</v>
       </c>
       <c r="B54" t="s">
         <v>142</v>
@@ -3810,7 +3798,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>259605</v>
+        <v>259597</v>
       </c>
       <c r="B55" t="s">
         <v>143</v>
@@ -3818,7 +3806,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>259603</v>
+        <v>259595</v>
       </c>
       <c r="B56" t="s">
         <v>144</v>
@@ -3826,7 +3814,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>259601</v>
+        <v>259593</v>
       </c>
       <c r="B57" t="s">
         <v>145</v>
@@ -3834,7 +3822,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>259599</v>
+        <v>259591</v>
       </c>
       <c r="B58" t="s">
         <v>146</v>
@@ -3842,49 +3830,17 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>259597</v>
+        <v>259585</v>
       </c>
       <c r="B59" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>259595</v>
-      </c>
-      <c r="B60" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>259593</v>
-      </c>
-      <c r="B61" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>259591</v>
-      </c>
-      <c r="B62" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>259585</v>
-      </c>
-      <c r="B63" t="s">
-        <v>151</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1 A64:A82">
+  <conditionalFormatting sqref="A60:A78 A1">
     <cfRule type="duplicateValues" dxfId="1" priority="148"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1 B64:B82">
+  <conditionalFormatting sqref="B60:B78 B1">
     <cfRule type="duplicateValues" dxfId="0" priority="150"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>